<commit_message>
Agregados valores faltantes de fila Sujeto5
</commit_message>
<xml_diff>
--- a/Efectividades.xlsx
+++ b/Efectividades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfc_2\Documents\Git\Clasificador-Bayesiano\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42619072-6F7C-4070-B7D7-2784C3D17BD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F946D2-D1A6-4ED4-B5E7-995C1E346D5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2670" yWindow="1425" windowWidth="12510" windowHeight="7875" xr2:uid="{6DF6BAD8-DCEE-4FDF-B5FC-1870D868E7E2}"/>
   </bookViews>
@@ -310,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -415,6 +415,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1263,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCAF7C7A-82F5-4FDE-94EB-09394C898A3F}">
-  <dimension ref="A1:BW30"/>
+  <dimension ref="A1:BW39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="AG16" sqref="AG16"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3127,42 +3130,42 @@
         <v>12</v>
       </c>
       <c r="AG14" s="26">
-        <v>0.95833330000000005</v>
+        <v>1</v>
       </c>
       <c r="AH14" s="27"/>
       <c r="AI14" s="9" t="s">
         <v>13</v>
       </c>
       <c r="AJ14" s="26">
-        <v>0.96875</v>
+        <v>1</v>
       </c>
       <c r="AK14" s="27"/>
       <c r="AL14" s="8" t="s">
         <v>12</v>
       </c>
       <c r="AM14" s="26">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AN14" s="27"/>
       <c r="AO14" s="9" t="s">
         <v>13</v>
       </c>
       <c r="AP14" s="26">
-        <v>0.84615300000000004</v>
+        <v>1</v>
       </c>
       <c r="AQ14" s="27"/>
       <c r="AR14" s="8" t="s">
         <v>12</v>
       </c>
       <c r="AS14" s="26">
-        <v>0.90740699999999996</v>
+        <v>0.925925</v>
       </c>
       <c r="AT14" s="27"/>
       <c r="AU14" s="9" t="s">
         <v>13</v>
       </c>
       <c r="AV14" s="26">
-        <v>0.84848400000000002</v>
+        <v>0.89393900000000004</v>
       </c>
       <c r="AW14" s="27"/>
       <c r="AX14" s="2"/>
@@ -3361,33 +3364,57 @@
       <c r="AE16" s="7">
         <v>18</v>
       </c>
-      <c r="AF16" s="5"/>
-      <c r="AG16" s="6"/>
+      <c r="AF16" s="5">
+        <v>46</v>
+      </c>
+      <c r="AG16" s="6">
+        <v>49</v>
+      </c>
       <c r="AH16" s="7">
         <v>12</v>
       </c>
-      <c r="AI16" s="6"/>
-      <c r="AJ16" s="6"/>
+      <c r="AI16" s="6">
+        <v>44</v>
+      </c>
+      <c r="AJ16" s="6">
+        <v>49</v>
+      </c>
       <c r="AK16" s="7">
         <v>16</v>
       </c>
-      <c r="AL16" s="5"/>
-      <c r="AM16" s="6"/>
+      <c r="AL16" s="5">
+        <v>23</v>
+      </c>
+      <c r="AM16" s="6">
+        <v>26</v>
+      </c>
       <c r="AN16" s="7">
         <v>10</v>
       </c>
-      <c r="AO16" s="6"/>
-      <c r="AP16" s="6"/>
+      <c r="AO16" s="6">
+        <v>26</v>
+      </c>
+      <c r="AP16" s="6">
+        <v>28</v>
+      </c>
       <c r="AQ16" s="7">
         <v>13</v>
       </c>
-      <c r="AR16" s="5"/>
-      <c r="AS16" s="6"/>
+      <c r="AR16" s="5">
+        <v>24</v>
+      </c>
+      <c r="AS16" s="6">
+        <v>41</v>
+      </c>
       <c r="AT16" s="7">
         <v>27</v>
       </c>
-      <c r="AU16" s="6"/>
-      <c r="AV16" s="6"/>
+      <c r="AU16" s="6">
+        <v>32</v>
+      </c>
+      <c r="AV16" s="6">
+        <v>39</v>
+      </c>
       <c r="AW16" s="7">
         <v>33</v>
       </c>
@@ -4274,7 +4301,7 @@
       <c r="E27" s="20"/>
       <c r="F27" s="24">
         <f>AVERAGE(C2,F2,I2,L2,O2,R2,U2,X2,AA2,AD2,AG2,AJ2,AM2,AP2,AS2,AV2,I5,L5,O5,R5,U5,X5,AA5,AD5,AG5,AJ5,AM5,AP5,AS5,AV5,O8,R8,U8,X8,AA8,AD8,AG8,AJ8,AM8,AP8,AS8,AV8,U11,X11,AA11,AD11,AG11,AJ11,AM11,AP11,AS11,AV11,AA14,AD14,AG14,AJ14,AM14,AP14,AS14,AV14,AG17,AJ17,AM17,AP17,AS17,AV17,AM20,AP20,AS20,AV20,AS23,AV23)</f>
-        <v>0.96925139305555552</v>
+        <v>0.97537273611111119</v>
       </c>
       <c r="G27" s="25"/>
       <c r="K27" s="20" t="s">
@@ -4299,7 +4326,7 @@
       <c r="E28" s="20"/>
       <c r="F28" s="21">
         <f>AVERAGE(B4,E4,H4,K4,N4,Q4,T4,W4,Z4,AC4,AF4,AI4,AL4,AO4,AR4,AU4,H7,K7,N7,Q7,T7,W7,Z7,AC7,AF7,AI7,AL7,AO7,AR7,AU7,N10,Q10,T10,W10,Z10,AC10,AF10,AI10,AL10,AO10,AR10,AU10,T13,W13,Z13,AC13,AF13,AI13,AL13,AO13,AR13,AU13,Z16,AC16,AF16,AI16,AL16,AO16,AR16,AU16,AF19,AI19,AL19,AO19,AR19,AU19,AL22,AO22,AR22,AU22,AR25,AU25)</f>
-        <v>33</v>
+        <v>32.950819672131146</v>
       </c>
       <c r="G28" s="21"/>
     </row>
@@ -4312,7 +4339,7 @@
       <c r="E29" s="20"/>
       <c r="F29" s="21">
         <f>AVERAGE(C4,F4,I4,L4,O4,R4,U4,X4,AA4,AD4,AG4,AJ4,AM4,AP4,AS4,AV4,I7,L7,O7,O10,R7,R10,U7,U10,U13,X7,X10,X13,AA7,AA10,AA13,AA16,AD7,AD10,AD13,AD16,AG7,AG10,AG13,AG16,AG19,AJ7,AJ10,AJ13,AJ16,AJ19,AM7,AM10,AM13,AM16,AM19,AM22,AP7,AP10,AP13,AP16,AP19,AP22,AS7,AS10,AS13,AS16,AS19,AS22,AS25,AV7,AV10,AV13,AV16,AV19,AV25)</f>
-        <v>41.870370370370374</v>
+        <v>41.55</v>
       </c>
       <c r="G29" s="21"/>
     </row>
@@ -4328,6 +4355,9 @@
         <v>42.75</v>
       </c>
       <c r="G30" s="21"/>
+    </row>
+    <row r="39" spans="47:47" x14ac:dyDescent="0.2">
+      <c r="AU39" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="140">

</xml_diff>

<commit_message>
Finalizada tabla de efectividades
</commit_message>
<xml_diff>
--- a/Efectividades.xlsx
+++ b/Efectividades.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfc_2\Documents\Git\Clasificador-Bayesiano\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F946D2-D1A6-4ED4-B5E7-995C1E346D5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9DCE23-3C42-47FC-B317-19CED41E8954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2670" yWindow="1425" windowWidth="12510" windowHeight="7875" xr2:uid="{6DF6BAD8-DCEE-4FDF-B5FC-1870D868E7E2}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -369,34 +368,16 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -408,16 +389,34 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1268,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCAF7C7A-82F5-4FDE-94EB-09394C898A3F}">
   <dimension ref="A1:BW39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1281,70 +1280,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:75" s="1" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="30" t="s">
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="30" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="30" t="s">
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="30" t="s">
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="30" t="s">
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="30" t="s">
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="30" t="s">
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
+      <c r="AO1" s="25"/>
+      <c r="AP1" s="25"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
-      <c r="AU1" s="31"/>
-      <c r="AV1" s="31"/>
-      <c r="AW1" s="32"/>
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="25"/>
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="25"/>
+      <c r="AW1" s="26"/>
       <c r="AX1" s="2"/>
       <c r="AY1" s="2"/>
       <c r="AZ1" s="2"/>
@@ -1373,124 +1372,124 @@
       <c r="BW1" s="2"/>
     </row>
     <row r="2" spans="1:75" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="27">
         <v>0.985294</v>
       </c>
-      <c r="D2" s="27"/>
+      <c r="D2" s="28"/>
       <c r="E2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="26">
+      <c r="F2" s="27">
         <v>0.98584899999999998</v>
       </c>
-      <c r="G2" s="27"/>
+      <c r="G2" s="28"/>
       <c r="H2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="26">
-        <v>1</v>
-      </c>
-      <c r="J2" s="27"/>
+      <c r="I2" s="27">
+        <v>1</v>
+      </c>
+      <c r="J2" s="28"/>
       <c r="K2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="26">
-        <v>1</v>
-      </c>
-      <c r="M2" s="27"/>
+      <c r="L2" s="27">
+        <v>1</v>
+      </c>
+      <c r="M2" s="28"/>
       <c r="N2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="26">
-        <v>1</v>
-      </c>
-      <c r="P2" s="27"/>
+      <c r="O2" s="27">
+        <v>1</v>
+      </c>
+      <c r="P2" s="28"/>
       <c r="Q2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="26">
-        <v>1</v>
-      </c>
-      <c r="S2" s="27"/>
+      <c r="R2" s="27">
+        <v>1</v>
+      </c>
+      <c r="S2" s="28"/>
       <c r="T2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="26">
-        <v>1</v>
-      </c>
-      <c r="V2" s="27"/>
+      <c r="U2" s="27">
+        <v>1</v>
+      </c>
+      <c r="V2" s="28"/>
       <c r="W2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="26">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="27"/>
+      <c r="X2" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="28"/>
       <c r="Z2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AA2" s="26">
+      <c r="AA2" s="27">
         <v>0.97959099999999999</v>
       </c>
-      <c r="AB2" s="27"/>
+      <c r="AB2" s="28"/>
       <c r="AC2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="AD2" s="26">
+      <c r="AD2" s="27">
         <v>0.95918300000000001</v>
       </c>
-      <c r="AE2" s="27"/>
+      <c r="AE2" s="28"/>
       <c r="AF2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AG2" s="26">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="27"/>
+      <c r="AG2" s="27">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="28"/>
       <c r="AI2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AJ2" s="26">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="27"/>
+      <c r="AJ2" s="27">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="28"/>
       <c r="AL2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AM2" s="26">
+      <c r="AM2" s="27">
         <v>0.98648599999999997</v>
       </c>
-      <c r="AN2" s="27"/>
+      <c r="AN2" s="28"/>
       <c r="AO2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AP2" s="26">
-        <v>1</v>
-      </c>
-      <c r="AQ2" s="27"/>
+      <c r="AP2" s="27">
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="28"/>
       <c r="AR2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AS2" s="26">
-        <v>1</v>
-      </c>
-      <c r="AT2" s="27"/>
+      <c r="AS2" s="27">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="28"/>
       <c r="AU2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AV2" s="26">
-        <v>1</v>
-      </c>
-      <c r="AW2" s="27"/>
+      <c r="AV2" s="27">
+        <v>1</v>
+      </c>
+      <c r="AW2" s="28"/>
     </row>
     <row r="3" spans="1:75" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="12" t="s">
         <v>10</v>
       </c>
@@ -1637,7 +1636,7 @@
       </c>
     </row>
     <row r="4" spans="1:75" s="1" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="5">
         <v>27</v>
       </c>
@@ -1810,7 +1809,7 @@
       <c r="BW4" s="2"/>
     </row>
     <row r="5" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="14"/>
@@ -1822,101 +1821,101 @@
       <c r="H5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="26">
-        <v>1</v>
-      </c>
-      <c r="J5" s="27"/>
+      <c r="I5" s="27">
+        <v>1</v>
+      </c>
+      <c r="J5" s="28"/>
       <c r="K5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="26">
-        <v>1</v>
-      </c>
-      <c r="M5" s="27"/>
+      <c r="L5" s="27">
+        <v>1</v>
+      </c>
+      <c r="M5" s="28"/>
       <c r="N5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="26">
-        <v>1</v>
-      </c>
-      <c r="P5" s="27"/>
+      <c r="O5" s="27">
+        <v>1</v>
+      </c>
+      <c r="P5" s="28"/>
       <c r="Q5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="R5" s="26">
-        <v>1</v>
-      </c>
-      <c r="S5" s="27"/>
+      <c r="R5" s="27">
+        <v>1</v>
+      </c>
+      <c r="S5" s="28"/>
       <c r="T5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="U5" s="26">
+      <c r="U5" s="27">
         <v>0.78662399999999999</v>
       </c>
-      <c r="V5" s="27"/>
+      <c r="V5" s="28"/>
       <c r="W5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="X5" s="26">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="27"/>
+      <c r="X5" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="28"/>
       <c r="Z5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AA5" s="26">
+      <c r="AA5" s="27">
         <v>0.95</v>
       </c>
-      <c r="AB5" s="27"/>
+      <c r="AB5" s="28"/>
       <c r="AC5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AD5" s="26">
+      <c r="AD5" s="27">
         <v>0.88561999999999996</v>
       </c>
-      <c r="AE5" s="27"/>
+      <c r="AE5" s="28"/>
       <c r="AF5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AG5" s="26">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="27"/>
+      <c r="AG5" s="27">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="28"/>
       <c r="AI5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AJ5" s="26">
-        <v>1</v>
-      </c>
-      <c r="AK5" s="27"/>
+      <c r="AJ5" s="27">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="28"/>
       <c r="AL5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AM5" s="26">
-        <v>1</v>
-      </c>
-      <c r="AN5" s="27"/>
+      <c r="AM5" s="27">
+        <v>1</v>
+      </c>
+      <c r="AN5" s="28"/>
       <c r="AO5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AP5" s="26">
+      <c r="AP5" s="27">
         <v>0.96078399999999997</v>
       </c>
-      <c r="AQ5" s="27"/>
+      <c r="AQ5" s="28"/>
       <c r="AR5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AS5" s="26">
+      <c r="AS5" s="27">
         <v>0.96</v>
       </c>
-      <c r="AT5" s="27"/>
+      <c r="AT5" s="28"/>
       <c r="AU5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AV5" s="26">
-        <v>1</v>
-      </c>
-      <c r="AW5" s="27"/>
+      <c r="AV5" s="27">
+        <v>1</v>
+      </c>
+      <c r="AW5" s="28"/>
       <c r="AX5" s="2"/>
       <c r="AY5" s="2"/>
       <c r="AZ5" s="2"/>
@@ -1945,7 +1944,7 @@
       <c r="BW5" s="2"/>
     </row>
     <row r="6" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="12"/>
       <c r="C6" s="11"/>
       <c r="D6" s="13"/>
@@ -2106,7 +2105,7 @@
       <c r="BW6" s="2"/>
     </row>
     <row r="7" spans="1:75" s="1" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="16"/>
       <c r="C7" s="17"/>
       <c r="D7" s="18"/>
@@ -2267,15 +2266,15 @@
       <c r="BW7" s="2"/>
     </row>
     <row r="8" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="21" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="14"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="30"/>
       <c r="H8" s="14"/>
       <c r="I8" s="10"/>
       <c r="J8" s="15"/>
@@ -2285,87 +2284,87 @@
       <c r="N8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="26">
-        <v>1</v>
-      </c>
-      <c r="P8" s="27"/>
+      <c r="O8" s="27">
+        <v>1</v>
+      </c>
+      <c r="P8" s="28"/>
       <c r="Q8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="R8" s="26">
+      <c r="R8" s="27">
         <v>0.98979499999999998</v>
       </c>
-      <c r="S8" s="27"/>
+      <c r="S8" s="28"/>
       <c r="T8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="U8" s="26">
+      <c r="U8" s="27">
         <v>0.99557499999999999</v>
       </c>
-      <c r="V8" s="27"/>
+      <c r="V8" s="28"/>
       <c r="W8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="X8" s="26">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="27"/>
+      <c r="X8" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="28"/>
       <c r="Z8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AA8" s="26">
-        <v>1</v>
-      </c>
-      <c r="AB8" s="27"/>
+      <c r="AA8" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="28"/>
       <c r="AC8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AD8" s="26">
-        <v>1</v>
-      </c>
-      <c r="AE8" s="27"/>
+      <c r="AD8" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="28"/>
       <c r="AF8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AG8" s="26">
-        <v>1</v>
-      </c>
-      <c r="AH8" s="27"/>
+      <c r="AG8" s="27">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="28"/>
       <c r="AI8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AJ8" s="26">
-        <v>1</v>
-      </c>
-      <c r="AK8" s="27"/>
+      <c r="AJ8" s="27">
+        <v>1</v>
+      </c>
+      <c r="AK8" s="28"/>
       <c r="AL8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AM8" s="26">
-        <v>1</v>
-      </c>
-      <c r="AN8" s="27"/>
+      <c r="AM8" s="27">
+        <v>1</v>
+      </c>
+      <c r="AN8" s="28"/>
       <c r="AO8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AP8" s="26">
-        <v>1</v>
-      </c>
-      <c r="AQ8" s="27"/>
+      <c r="AP8" s="27">
+        <v>1</v>
+      </c>
+      <c r="AQ8" s="28"/>
       <c r="AR8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AS8" s="26">
-        <v>1</v>
-      </c>
-      <c r="AT8" s="27"/>
+      <c r="AS8" s="27">
+        <v>1</v>
+      </c>
+      <c r="AT8" s="28"/>
       <c r="AU8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AV8" s="26">
-        <v>1</v>
-      </c>
-      <c r="AW8" s="27"/>
+      <c r="AV8" s="27">
+        <v>1</v>
+      </c>
+      <c r="AW8" s="28"/>
       <c r="AX8" s="2"/>
       <c r="AY8" s="2"/>
       <c r="AZ8" s="2"/>
@@ -2394,7 +2393,7 @@
       <c r="BW8" s="2"/>
     </row>
     <row r="9" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="12"/>
       <c r="C9" s="11"/>
       <c r="D9" s="13"/>
@@ -2543,7 +2542,7 @@
       <c r="BW9" s="2"/>
     </row>
     <row r="10" spans="1:75" s="1" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="16"/>
       <c r="C10" s="17"/>
       <c r="D10" s="18"/>
@@ -2692,21 +2691,21 @@
       <c r="BW10" s="2"/>
     </row>
     <row r="11" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="14"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="29"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="32"/>
       <c r="E11" s="10"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="30"/>
       <c r="H11" s="14"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="23"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="30"/>
       <c r="K11" s="10"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="23"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="30"/>
       <c r="N11" s="14"/>
       <c r="O11" s="10"/>
       <c r="P11" s="15"/>
@@ -2716,73 +2715,73 @@
       <c r="T11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="U11" s="26">
-        <v>1</v>
-      </c>
-      <c r="V11" s="27"/>
+      <c r="U11" s="27">
+        <v>1</v>
+      </c>
+      <c r="V11" s="28"/>
       <c r="W11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="X11" s="26">
+      <c r="X11" s="27">
         <v>0.91666599999999998</v>
       </c>
-      <c r="Y11" s="27"/>
+      <c r="Y11" s="28"/>
       <c r="Z11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AA11" s="26">
-        <v>1</v>
-      </c>
-      <c r="AB11" s="27"/>
+      <c r="AA11" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="28"/>
       <c r="AC11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AD11" s="26">
-        <v>1</v>
-      </c>
-      <c r="AE11" s="27"/>
+      <c r="AD11" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="28"/>
       <c r="AF11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AG11" s="26">
-        <v>1</v>
-      </c>
-      <c r="AH11" s="27"/>
+      <c r="AG11" s="27">
+        <v>1</v>
+      </c>
+      <c r="AH11" s="28"/>
       <c r="AI11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AJ11" s="26">
-        <v>1</v>
-      </c>
-      <c r="AK11" s="27"/>
+      <c r="AJ11" s="27">
+        <v>1</v>
+      </c>
+      <c r="AK11" s="28"/>
       <c r="AL11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AM11" s="26">
-        <v>1</v>
-      </c>
-      <c r="AN11" s="27"/>
+      <c r="AM11" s="27">
+        <v>1</v>
+      </c>
+      <c r="AN11" s="28"/>
       <c r="AO11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AP11" s="26">
+      <c r="AP11" s="27">
         <v>0.97916599999999998</v>
       </c>
-      <c r="AQ11" s="27"/>
+      <c r="AQ11" s="28"/>
       <c r="AR11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AS11" s="26">
-        <v>1</v>
-      </c>
-      <c r="AT11" s="27"/>
+      <c r="AS11" s="27">
+        <v>1</v>
+      </c>
+      <c r="AT11" s="28"/>
       <c r="AU11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AV11" s="26">
-        <v>1</v>
-      </c>
-      <c r="AW11" s="27"/>
+      <c r="AV11" s="27">
+        <v>1</v>
+      </c>
+      <c r="AW11" s="28"/>
       <c r="AX11" s="2"/>
       <c r="AY11" s="2"/>
       <c r="AZ11" s="2"/>
@@ -2811,7 +2810,7 @@
       <c r="BW11" s="2"/>
     </row>
     <row r="12" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="34"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="12"/>
       <c r="C12" s="11"/>
       <c r="D12" s="13"/>
@@ -2948,7 +2947,7 @@
       <c r="BW12" s="2"/>
     </row>
     <row r="13" spans="1:75" s="1" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="16"/>
       <c r="C13" s="17"/>
       <c r="D13" s="18"/>
@@ -3085,27 +3084,27 @@
       <c r="BW13" s="2"/>
     </row>
     <row r="14" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="21" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="14"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="23"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="23"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="30"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="23"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="30"/>
       <c r="K14" s="10"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="23"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="30"/>
       <c r="N14" s="14"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="23"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="30"/>
       <c r="Q14" s="10"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="23"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="30"/>
       <c r="T14" s="14"/>
       <c r="U14" s="10"/>
       <c r="V14" s="15"/>
@@ -3115,59 +3114,59 @@
       <c r="Z14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AA14" s="26">
-        <v>1</v>
-      </c>
-      <c r="AB14" s="27"/>
+      <c r="AA14" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="28"/>
       <c r="AC14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AD14" s="26">
-        <v>1</v>
-      </c>
-      <c r="AE14" s="27"/>
+      <c r="AD14" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE14" s="28"/>
       <c r="AF14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AG14" s="26">
-        <v>1</v>
-      </c>
-      <c r="AH14" s="27"/>
+      <c r="AG14" s="27">
+        <v>1</v>
+      </c>
+      <c r="AH14" s="28"/>
       <c r="AI14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AJ14" s="26">
-        <v>1</v>
-      </c>
-      <c r="AK14" s="27"/>
+      <c r="AJ14" s="27">
+        <v>1</v>
+      </c>
+      <c r="AK14" s="28"/>
       <c r="AL14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AM14" s="26">
-        <v>1</v>
-      </c>
-      <c r="AN14" s="27"/>
+      <c r="AM14" s="27">
+        <v>1</v>
+      </c>
+      <c r="AN14" s="28"/>
       <c r="AO14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AP14" s="26">
-        <v>1</v>
-      </c>
-      <c r="AQ14" s="27"/>
+      <c r="AP14" s="27">
+        <v>1</v>
+      </c>
+      <c r="AQ14" s="28"/>
       <c r="AR14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AS14" s="26">
+      <c r="AS14" s="27">
         <v>0.925925</v>
       </c>
-      <c r="AT14" s="27"/>
+      <c r="AT14" s="28"/>
       <c r="AU14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AV14" s="26">
+      <c r="AV14" s="27">
         <v>0.89393900000000004</v>
       </c>
-      <c r="AW14" s="27"/>
+      <c r="AW14" s="28"/>
       <c r="AX14" s="2"/>
       <c r="AY14" s="2"/>
       <c r="AZ14" s="2"/>
@@ -3196,7 +3195,7 @@
       <c r="BW14" s="2"/>
     </row>
     <row r="15" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="34"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="12"/>
       <c r="C15" s="11"/>
       <c r="D15" s="13"/>
@@ -3321,7 +3320,7 @@
       <c r="BW15" s="2"/>
     </row>
     <row r="16" spans="1:75" s="1" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="16"/>
       <c r="C16" s="17"/>
       <c r="D16" s="18"/>
@@ -3446,33 +3445,33 @@
       <c r="BW16" s="2"/>
     </row>
     <row r="17" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="21" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="14"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="23"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="23"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="30"/>
       <c r="H17" s="14"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="23"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="30"/>
       <c r="K17" s="10"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="23"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="30"/>
       <c r="N17" s="14"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="23"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="30"/>
       <c r="Q17" s="10"/>
-      <c r="R17" s="22"/>
-      <c r="S17" s="23"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="30"/>
       <c r="T17" s="14"/>
-      <c r="U17" s="22"/>
-      <c r="V17" s="23"/>
+      <c r="U17" s="29"/>
+      <c r="V17" s="30"/>
       <c r="W17" s="10"/>
-      <c r="X17" s="22"/>
-      <c r="Y17" s="23"/>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="30"/>
       <c r="Z17" s="14"/>
       <c r="AA17" s="10"/>
       <c r="AB17" s="15"/>
@@ -3482,45 +3481,45 @@
       <c r="AF17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AG17" s="26">
-        <v>0.98979499999999998</v>
-      </c>
-      <c r="AH17" s="27"/>
+      <c r="AG17" s="27">
+        <v>1</v>
+      </c>
+      <c r="AH17" s="28"/>
       <c r="AI17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AJ17" s="26">
-        <v>0.99264699999999995</v>
-      </c>
-      <c r="AK17" s="27"/>
+      <c r="AJ17" s="27">
+        <v>1</v>
+      </c>
+      <c r="AK17" s="28"/>
       <c r="AL17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AM17" s="26">
-        <v>0.83333299999999999</v>
-      </c>
-      <c r="AN17" s="27"/>
+      <c r="AM17" s="27">
+        <v>0.98333300000000001</v>
+      </c>
+      <c r="AN17" s="28"/>
       <c r="AO17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AP17" s="26">
-        <v>0.90476100000000004</v>
-      </c>
-      <c r="AQ17" s="27"/>
+      <c r="AP17" s="27">
+        <v>1</v>
+      </c>
+      <c r="AQ17" s="28"/>
       <c r="AR17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AS17" s="26">
-        <v>0.91666599999999998</v>
-      </c>
-      <c r="AT17" s="27"/>
+      <c r="AS17" s="27">
+        <v>0.97916599999999998</v>
+      </c>
+      <c r="AT17" s="28"/>
       <c r="AU17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AV17" s="26">
-        <v>0.84615300000000004</v>
-      </c>
-      <c r="AW17" s="27"/>
+      <c r="AV17" s="27">
+        <v>1</v>
+      </c>
+      <c r="AW17" s="28"/>
       <c r="AX17" s="2"/>
       <c r="AY17" s="2"/>
       <c r="AZ17" s="2"/>
@@ -3549,7 +3548,7 @@
       <c r="BW17" s="2"/>
     </row>
     <row r="18" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="12"/>
       <c r="C18" s="11"/>
       <c r="D18" s="13"/>
@@ -3662,7 +3661,7 @@
       <c r="BW18" s="2"/>
     </row>
     <row r="19" spans="1:75" s="1" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="16"/>
       <c r="C19" s="17"/>
       <c r="D19" s="18"/>
@@ -3693,33 +3692,57 @@
       <c r="AC19" s="17"/>
       <c r="AD19" s="17"/>
       <c r="AE19" s="18"/>
-      <c r="AF19" s="5"/>
-      <c r="AG19" s="6"/>
+      <c r="AF19" s="5">
+        <v>39</v>
+      </c>
+      <c r="AG19" s="6">
+        <v>56</v>
+      </c>
       <c r="AH19" s="7">
+        <v>33</v>
+      </c>
+      <c r="AI19" s="6">
+        <v>24</v>
+      </c>
+      <c r="AJ19" s="6">
         <v>49</v>
       </c>
-      <c r="AI19" s="6"/>
-      <c r="AJ19" s="6"/>
       <c r="AK19" s="7">
         <v>68</v>
       </c>
-      <c r="AL19" s="5"/>
-      <c r="AM19" s="6"/>
+      <c r="AL19" s="5">
+        <v>38</v>
+      </c>
+      <c r="AM19" s="6">
+        <v>49</v>
+      </c>
       <c r="AN19" s="7">
         <v>30</v>
       </c>
-      <c r="AO19" s="6"/>
-      <c r="AP19" s="6"/>
+      <c r="AO19" s="6">
+        <v>38</v>
+      </c>
+      <c r="AP19" s="6">
+        <v>49</v>
+      </c>
       <c r="AQ19" s="7">
         <v>21</v>
       </c>
-      <c r="AR19" s="5"/>
-      <c r="AS19" s="6"/>
+      <c r="AR19" s="5">
+        <v>42</v>
+      </c>
+      <c r="AS19" s="6">
+        <v>49</v>
+      </c>
       <c r="AT19" s="7">
         <v>24</v>
       </c>
-      <c r="AU19" s="6"/>
-      <c r="AV19" s="6"/>
+      <c r="AU19" s="6">
+        <v>46</v>
+      </c>
+      <c r="AV19" s="6">
+        <v>49</v>
+      </c>
       <c r="AW19" s="7">
         <v>13</v>
       </c>
@@ -3751,39 +3774,39 @@
       <c r="BW19" s="2"/>
     </row>
     <row r="20" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="14"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="23"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="23"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="30"/>
       <c r="H20" s="14"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="23"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="30"/>
       <c r="K20" s="10"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="23"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="30"/>
       <c r="N20" s="14"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="23"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="30"/>
       <c r="Q20" s="10"/>
-      <c r="R20" s="22"/>
-      <c r="S20" s="23"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="30"/>
       <c r="T20" s="14"/>
-      <c r="U20" s="22"/>
-      <c r="V20" s="23"/>
+      <c r="U20" s="29"/>
+      <c r="V20" s="30"/>
       <c r="W20" s="10"/>
-      <c r="X20" s="22"/>
-      <c r="Y20" s="23"/>
+      <c r="X20" s="29"/>
+      <c r="Y20" s="30"/>
       <c r="Z20" s="14"/>
-      <c r="AA20" s="22"/>
-      <c r="AB20" s="23"/>
+      <c r="AA20" s="29"/>
+      <c r="AB20" s="30"/>
       <c r="AC20" s="10"/>
-      <c r="AD20" s="22"/>
-      <c r="AE20" s="23"/>
+      <c r="AD20" s="29"/>
+      <c r="AE20" s="30"/>
       <c r="AF20" s="14"/>
       <c r="AG20" s="10"/>
       <c r="AH20" s="15"/>
@@ -3793,31 +3816,31 @@
       <c r="AL20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AM20" s="26">
-        <v>0.98979499999999998</v>
-      </c>
-      <c r="AN20" s="27"/>
+      <c r="AM20" s="27">
+        <v>1</v>
+      </c>
+      <c r="AN20" s="28"/>
       <c r="AO20" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AP20" s="26">
-        <v>0.98936100000000005</v>
-      </c>
-      <c r="AQ20" s="27"/>
+      <c r="AP20" s="27">
+        <v>1</v>
+      </c>
+      <c r="AQ20" s="28"/>
       <c r="AR20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AS20" s="26">
-        <v>0.96875</v>
-      </c>
-      <c r="AT20" s="27"/>
+      <c r="AS20" s="27">
+        <v>0.98958299999999999</v>
+      </c>
+      <c r="AT20" s="28"/>
       <c r="AU20" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AV20" s="26">
-        <v>1</v>
-      </c>
-      <c r="AW20" s="27"/>
+      <c r="AV20" s="27">
+        <v>1</v>
+      </c>
+      <c r="AW20" s="28"/>
       <c r="AX20" s="2"/>
       <c r="AY20" s="2"/>
       <c r="AZ20" s="2"/>
@@ -3846,7 +3869,7 @@
       <c r="BW20" s="2"/>
     </row>
     <row r="21" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="34"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="12"/>
       <c r="C21" s="11"/>
       <c r="D21" s="13"/>
@@ -3947,7 +3970,7 @@
       <c r="BW21" s="2"/>
     </row>
     <row r="22" spans="1:75" s="1" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="16"/>
       <c r="C22" s="17"/>
       <c r="D22" s="18"/>
@@ -3984,18 +4007,30 @@
       <c r="AI22" s="17"/>
       <c r="AJ22" s="17"/>
       <c r="AK22" s="18"/>
-      <c r="AL22" s="5"/>
-      <c r="AM22" s="6"/>
+      <c r="AL22" s="5">
+        <v>30</v>
+      </c>
+      <c r="AM22" s="6">
+        <v>49</v>
+      </c>
       <c r="AN22" s="7">
         <v>49</v>
       </c>
-      <c r="AO22" s="6"/>
-      <c r="AP22" s="6"/>
+      <c r="AO22" s="6">
+        <v>38</v>
+      </c>
+      <c r="AP22" s="6">
+        <v>49</v>
+      </c>
       <c r="AQ22" s="7">
         <v>47</v>
       </c>
-      <c r="AR22" s="5"/>
-      <c r="AS22" s="6"/>
+      <c r="AR22" s="5">
+        <v>31</v>
+      </c>
+      <c r="AS22" s="6">
+        <v>38</v>
+      </c>
       <c r="AT22" s="7">
         <v>48</v>
       </c>
@@ -4036,45 +4071,45 @@
       <c r="BW22" s="2"/>
     </row>
     <row r="23" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="21" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="14"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="23"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
       <c r="E23" s="10"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="23"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="30"/>
       <c r="H23" s="14"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="23"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="30"/>
       <c r="K23" s="10"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="23"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="30"/>
       <c r="N23" s="14"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="23"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="30"/>
       <c r="Q23" s="10"/>
-      <c r="R23" s="22"/>
-      <c r="S23" s="23"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="30"/>
       <c r="T23" s="14"/>
-      <c r="U23" s="22"/>
-      <c r="V23" s="23"/>
+      <c r="U23" s="29"/>
+      <c r="V23" s="30"/>
       <c r="W23" s="10"/>
-      <c r="X23" s="22"/>
-      <c r="Y23" s="23"/>
+      <c r="X23" s="29"/>
+      <c r="Y23" s="30"/>
       <c r="Z23" s="14"/>
-      <c r="AA23" s="22"/>
-      <c r="AB23" s="23"/>
+      <c r="AA23" s="29"/>
+      <c r="AB23" s="30"/>
       <c r="AC23" s="10"/>
-      <c r="AD23" s="22"/>
-      <c r="AE23" s="23"/>
+      <c r="AD23" s="29"/>
+      <c r="AE23" s="30"/>
       <c r="AF23" s="14"/>
-      <c r="AG23" s="22"/>
-      <c r="AH23" s="23"/>
+      <c r="AG23" s="29"/>
+      <c r="AH23" s="30"/>
       <c r="AI23" s="10"/>
-      <c r="AJ23" s="22"/>
-      <c r="AK23" s="23"/>
+      <c r="AJ23" s="29"/>
+      <c r="AK23" s="30"/>
       <c r="AL23" s="14"/>
       <c r="AM23" s="10"/>
       <c r="AN23" s="15"/>
@@ -4084,17 +4119,17 @@
       <c r="AR23" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AS23" s="26">
-        <v>0.88235200000000003</v>
-      </c>
-      <c r="AT23" s="27"/>
+      <c r="AS23" s="27">
+        <v>0.97058800000000001</v>
+      </c>
+      <c r="AT23" s="28"/>
       <c r="AU23" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AV23" s="26">
-        <v>0.77272700000000005</v>
-      </c>
-      <c r="AW23" s="27"/>
+      <c r="AV23" s="27">
+        <v>0.94117600000000001</v>
+      </c>
+      <c r="AW23" s="28"/>
       <c r="AX23" s="2"/>
       <c r="AY23" s="2"/>
       <c r="AZ23" s="2"/>
@@ -4123,7 +4158,7 @@
       <c r="BW23" s="2"/>
     </row>
     <row r="24" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="12"/>
       <c r="C24" s="11"/>
       <c r="D24" s="13"/>
@@ -4212,7 +4247,7 @@
       <c r="BW24" s="2"/>
     </row>
     <row r="25" spans="1:75" s="1" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="16"/>
       <c r="C25" s="17"/>
       <c r="D25" s="18"/>
@@ -4255,13 +4290,21 @@
       <c r="AO25" s="17"/>
       <c r="AP25" s="17"/>
       <c r="AQ25" s="18"/>
-      <c r="AR25" s="5"/>
-      <c r="AS25" s="6"/>
+      <c r="AR25" s="5">
+        <v>41</v>
+      </c>
+      <c r="AS25" s="6">
+        <v>49</v>
+      </c>
       <c r="AT25" s="7">
         <v>17</v>
       </c>
-      <c r="AU25" s="6"/>
-      <c r="AV25" s="6"/>
+      <c r="AU25" s="6">
+        <v>40</v>
+      </c>
+      <c r="AV25" s="6">
+        <v>49</v>
+      </c>
       <c r="AW25" s="7">
         <v>22</v>
       </c>
@@ -4293,74 +4336,190 @@
       <c r="BW25" s="2"/>
     </row>
     <row r="27" spans="1:75" x14ac:dyDescent="0.2">
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="24">
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="33">
         <f>AVERAGE(C2,F2,I2,L2,O2,R2,U2,X2,AA2,AD2,AG2,AJ2,AM2,AP2,AS2,AV2,I5,L5,O5,R5,U5,X5,AA5,AD5,AG5,AJ5,AM5,AP5,AS5,AV5,O8,R8,U8,X8,AA8,AD8,AG8,AJ8,AM8,AP8,AS8,AV8,U11,X11,AA11,AD11,AG11,AJ11,AM11,AP11,AS11,AV11,AA14,AD14,AG14,AJ14,AM14,AP14,AS14,AV14,AG17,AJ17,AM17,AP17,AS17,AV17,AM20,AP20,AS20,AV20,AS23,AV23)</f>
-        <v>0.97537273611111119</v>
-      </c>
-      <c r="G27" s="25"/>
-      <c r="K27" s="20" t="s">
+        <v>0.98617143055555567</v>
+      </c>
+      <c r="G27" s="34"/>
+      <c r="K27" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="24">
+      <c r="L27" s="35"/>
+      <c r="M27" s="35"/>
+      <c r="N27" s="35"/>
+      <c r="O27" s="35"/>
+      <c r="P27" s="35"/>
+      <c r="Q27" s="33">
         <v>0.938967</v>
       </c>
-      <c r="R27" s="25"/>
+      <c r="R27" s="34"/>
     </row>
     <row r="28" spans="1:75" x14ac:dyDescent="0.2">
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="21">
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="36">
         <f>AVERAGE(B4,E4,H4,K4,N4,Q4,T4,W4,Z4,AC4,AF4,AI4,AL4,AO4,AR4,AU4,H7,K7,N7,Q7,T7,W7,Z7,AC7,AF7,AI7,AL7,AO7,AR7,AU7,N10,Q10,T10,W10,Z10,AC10,AF10,AI10,AL10,AO10,AR10,AU10,T13,W13,Z13,AC13,AF13,AI13,AL13,AO13,AR13,AU13,Z16,AC16,AF16,AI16,AL16,AO16,AR16,AU16,AF19,AI19,AL19,AO19,AR19,AU19,AL22,AO22,AR22,AU22,AR25,AU25)</f>
-        <v>32.950819672131146</v>
-      </c>
-      <c r="G28" s="21"/>
+        <v>33.569444444444443</v>
+      </c>
+      <c r="G28" s="36"/>
     </row>
     <row r="29" spans="1:75" x14ac:dyDescent="0.2">
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="21">
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="36">
         <f>AVERAGE(C4,F4,I4,L4,O4,R4,U4,X4,AA4,AD4,AG4,AJ4,AM4,AP4,AS4,AV4,I7,L7,O7,O10,R7,R10,U7,U10,U13,X7,X10,X13,AA7,AA10,AA13,AA16,AD7,AD10,AD13,AD16,AG7,AG10,AG13,AG16,AG19,AJ7,AJ10,AJ13,AJ16,AJ19,AM7,AM10,AM13,AM16,AM19,AM22,AP7,AP10,AP13,AP16,AP19,AP22,AS7,AS10,AS13,AS16,AS19,AS22,AS25,AV7,AV10,AV13,AV16,AV19,AV25)</f>
-        <v>41.55</v>
-      </c>
-      <c r="G29" s="21"/>
+        <v>42.647887323943664</v>
+      </c>
+      <c r="G29" s="36"/>
     </row>
     <row r="30" spans="1:75" x14ac:dyDescent="0.2">
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="21">
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="36">
         <f>AVERAGE(D4,G4,J4,J7,M4,M7,P4,P7,P10,S4,S7,S10,V4,V7,V10,V13,Y4,Y7,Y10,Y13,AB4,AB7,AB10,AB13,AB16,AE4,AE7,AE10,AE13,AE16,AH4,AH7,AH10,AH13,AH16,AH19,AK4,AK7,AK10,AK13,AK16,AK19,AN4,AN7,AN10,AN13,AN16,AN19,AN22,AQ4,AQ7,AQ10,AQ13,AQ16,AQ19,AQ22,AT4,AT7,AT10,AT13,AT16,AT19,AT22,AT25,AW4,AW7,AW10,AW13,AW16,AW19,AW22,AW25)</f>
-        <v>42.75</v>
-      </c>
-      <c r="G30" s="21"/>
+        <v>42.527777777777779</v>
+      </c>
+      <c r="G30" s="36"/>
     </row>
     <row r="39" spans="47:47" x14ac:dyDescent="0.2">
-      <c r="AU39" s="36"/>
+      <c r="AU39" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="140">
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="K27:P27"/>
+    <mergeCell ref="AS23:AT23"/>
+    <mergeCell ref="AV23:AW23"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="AA23:AB23"/>
+    <mergeCell ref="AD23:AE23"/>
+    <mergeCell ref="AG23:AH23"/>
+    <mergeCell ref="AJ23:AK23"/>
+    <mergeCell ref="AM20:AN20"/>
+    <mergeCell ref="AP20:AQ20"/>
+    <mergeCell ref="AS20:AT20"/>
+    <mergeCell ref="AV20:AW20"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="X20:Y20"/>
+    <mergeCell ref="AA20:AB20"/>
+    <mergeCell ref="AD20:AE20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="X17:Y17"/>
+    <mergeCell ref="AG17:AH17"/>
+    <mergeCell ref="AM14:AN14"/>
+    <mergeCell ref="AP14:AQ14"/>
+    <mergeCell ref="AS14:AT14"/>
+    <mergeCell ref="AV14:AW14"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="AA14:AB14"/>
+    <mergeCell ref="AD14:AE14"/>
+    <mergeCell ref="AG14:AH14"/>
+    <mergeCell ref="AJ14:AK14"/>
+    <mergeCell ref="AM17:AN17"/>
+    <mergeCell ref="AP17:AQ17"/>
+    <mergeCell ref="AS17:AT17"/>
+    <mergeCell ref="AV17:AW17"/>
+    <mergeCell ref="AJ17:AK17"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="X11:Y11"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AD11:AE11"/>
+    <mergeCell ref="AG11:AH11"/>
+    <mergeCell ref="AM8:AN8"/>
+    <mergeCell ref="AP8:AQ8"/>
+    <mergeCell ref="AS8:AT8"/>
+    <mergeCell ref="AV8:AW8"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="X8:Y8"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="AD8:AE8"/>
+    <mergeCell ref="AG8:AH8"/>
+    <mergeCell ref="AJ8:AK8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="AM11:AN11"/>
+    <mergeCell ref="AP11:AQ11"/>
+    <mergeCell ref="AS11:AT11"/>
+    <mergeCell ref="AV11:AW11"/>
+    <mergeCell ref="AJ11:AK11"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AJ5:AK5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AP5:AQ5"/>
+    <mergeCell ref="AS5:AT5"/>
+    <mergeCell ref="AV5:AW5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="AL1:AQ1"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="AR1:AW1"/>
+    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="Z1:AE1"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF1:AK1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AJ2:AK2"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="T1:Y1"/>
@@ -4385,122 +4544,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="F14:G14"/>
-    <mergeCell ref="AL1:AQ1"/>
-    <mergeCell ref="AM2:AN2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="AR1:AW1"/>
-    <mergeCell ref="AS2:AT2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="Z1:AE1"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF1:AK1"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AJ5:AK5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AP5:AQ5"/>
-    <mergeCell ref="AS5:AT5"/>
-    <mergeCell ref="AV5:AW5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="AS8:AT8"/>
-    <mergeCell ref="AV8:AW8"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="X8:Y8"/>
-    <mergeCell ref="AA8:AB8"/>
-    <mergeCell ref="AD8:AE8"/>
-    <mergeCell ref="AG8:AH8"/>
-    <mergeCell ref="AJ8:AK8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="AM11:AN11"/>
-    <mergeCell ref="AP11:AQ11"/>
-    <mergeCell ref="AS11:AT11"/>
-    <mergeCell ref="AV11:AW11"/>
-    <mergeCell ref="AJ11:AK11"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="X11:Y11"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="AD11:AE11"/>
-    <mergeCell ref="AG11:AH11"/>
-    <mergeCell ref="AM8:AN8"/>
-    <mergeCell ref="AP8:AQ8"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="X17:Y17"/>
-    <mergeCell ref="AG17:AH17"/>
-    <mergeCell ref="AM14:AN14"/>
-    <mergeCell ref="AP14:AQ14"/>
-    <mergeCell ref="AS14:AT14"/>
-    <mergeCell ref="AV14:AW14"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="AA14:AB14"/>
-    <mergeCell ref="AD14:AE14"/>
-    <mergeCell ref="AG14:AH14"/>
-    <mergeCell ref="AJ14:AK14"/>
-    <mergeCell ref="AM17:AN17"/>
-    <mergeCell ref="AP17:AQ17"/>
-    <mergeCell ref="AS17:AT17"/>
-    <mergeCell ref="AV17:AW17"/>
-    <mergeCell ref="AJ17:AK17"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="AM20:AN20"/>
-    <mergeCell ref="AP20:AQ20"/>
-    <mergeCell ref="AS20:AT20"/>
-    <mergeCell ref="AV20:AW20"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="U20:V20"/>
-    <mergeCell ref="X20:Y20"/>
-    <mergeCell ref="AA20:AB20"/>
-    <mergeCell ref="AD20:AE20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="K27:P27"/>
-    <mergeCell ref="AS23:AT23"/>
-    <mergeCell ref="AV23:AW23"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="AA23:AB23"/>
-    <mergeCell ref="AD23:AE23"/>
-    <mergeCell ref="AG23:AH23"/>
-    <mergeCell ref="AJ23:AK23"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="F27:G27"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="AX2:XFD2 A2:AE2">

</xml_diff>